<commit_message>
Start emulator and complete clock module
</commit_message>
<xml_diff>
--- a/docs/Labels.xlsx
+++ b/docs/Labels.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t xml:space="preserve">C
 I
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve">Lower ALU Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper MAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower MAR</t>
   </si>
 </sst>
 </file>
@@ -145,6 +151,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -165,6 +172,7 @@
       <sz val="4.5"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -297,12 +305,12 @@
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="390" zoomScaleNormal="390" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+      <selection pane="topLeft" activeCell="U25" activeCellId="0" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="5.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="1.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="1.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="2.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="12" style="1" width="1.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="22" style="1" width="11.52"/>
@@ -762,41 +770,133 @@
       <c r="T22" s="6"/>
       <c r="U22" s="7"/>
     </row>
+    <row r="24" customFormat="false" ht="5.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="L24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+    </row>
     <row r="25" customFormat="false" ht="5.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
-      <c r="E25" s="0"/>
-      <c r="F25" s="0"/>
-      <c r="G25" s="0"/>
-      <c r="H25" s="0"/>
-      <c r="I25" s="0"/>
-      <c r="J25" s="0"/>
+      <c r="A25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="7"/>
+      <c r="L25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q25" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="R25" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="S25" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="U25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="5.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="0"/>
-      <c r="F26" s="0"/>
-      <c r="G26" s="0"/>
-      <c r="H26" s="0"/>
-      <c r="I26" s="0"/>
-      <c r="J26" s="0"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="7"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="5.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
-      <c r="E27" s="0"/>
-      <c r="F27" s="0"/>
-      <c r="G27" s="0"/>
-      <c r="H27" s="0"/>
-      <c r="I27" s="0"/>
-      <c r="J27" s="0"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="7"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="5.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
@@ -907,7 +1007,7 @@
       <c r="J40" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="76">
+  <mergeCells count="98">
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -984,6 +1084,28 @@
     <mergeCell ref="S20:S22"/>
     <mergeCell ref="T20:T22"/>
     <mergeCell ref="U20:U22"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="L24:U24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="M25:M27"/>
+    <mergeCell ref="N25:N27"/>
+    <mergeCell ref="O25:O27"/>
+    <mergeCell ref="P25:P27"/>
+    <mergeCell ref="Q25:Q27"/>
+    <mergeCell ref="R25:R27"/>
+    <mergeCell ref="S25:S27"/>
+    <mergeCell ref="T25:T27"/>
+    <mergeCell ref="U25:U27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>